<commit_message>
add DESCRIPTION for ui.R/server.R debug console in browser add helpers.R for plotting function fine-tuning of server.R und ui.R !!! one thing only missing in helpers.R... waiting for forum reply
</commit_message>
<xml_diff>
--- a/data/adac-unfallgeschehen.xlsx
+++ b/data/adac-unfallgeschehen.xlsx
@@ -4896,10 +4896,10 @@
     <t>F-less18</t>
   </si>
   <si>
-    <t>M-18-21</t>
-  </si>
-  <si>
-    <t>F-18-21</t>
+    <t>M-from18to21</t>
+  </si>
+  <si>
+    <t>F-from18to21</t>
   </si>
   <si>
     <t>M-21-25</t>
@@ -9388,7 +9388,7 @@
   <dimension ref="A1:S18"/>
   <sheetViews>
     <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="E19" activeCellId="0" sqref="E19"/>
+      <selection pane="topLeft" activeCell="G2" activeCellId="0" sqref="G2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.8"/>

</xml_diff>